<commit_message>
added configs X-ray receiver
</commit_message>
<xml_diff>
--- a/GameData/WarpPlugin/Parts/Microwave/BeamGenerators/FreeElectronLaser/KSPIE Brandwidths.xlsx
+++ b/GameData/WarpPlugin/Parts/Microwave/BeamGenerators/FreeElectronLaser/KSPIE Brandwidths.xlsx
@@ -537,7 +537,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +829,7 @@
         <v>16</v>
       </c>
       <c r="E17">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F17">
         <v>41</v>
@@ -846,7 +846,7 @@
         <v>10</v>
       </c>
       <c r="E18">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>38</v>

</xml_diff>